<commit_message>
Ajuste de escaleta Mat 8 tema 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA MA_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA MA_08_07_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
     <author>Edgar Josué Malagón Montaña</author>
   </authors>
   <commentList>
-    <comment ref="G10" authorId="0" shapeId="0">
+    <comment ref="G9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N11" authorId="0" shapeId="0">
+    <comment ref="N10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G23" authorId="0" shapeId="0">
+    <comment ref="G21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H30" authorId="0" shapeId="0">
+    <comment ref="H28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="242">
   <si>
     <t>Asignatura</t>
   </si>
@@ -513,21 +513,6 @@
     <t>En las imágenes se ubican tablas que relacionan las variables x y y.  Sugerir al menos cinco ejercicios. Las alternativas de respuestas son: Es función; No es función.</t>
   </si>
   <si>
-    <t>Relaciona funciones con su expresión algebraica</t>
-  </si>
-  <si>
-    <t>Actividad que permite relacionar a una expresión algebraica un elemento de su domnio</t>
-  </si>
-  <si>
-    <t>En las imágenes de la izquierda sugerir las expresiones x/2  + 2; y + 1/y; =RAIZ(2x); Raizcúbica(x)/3; (a + 4)EXP(4); xEXP(2) + 10.
-En las alternativas de la derecha escribir: La mitad de un número más 2. 
-La suma de un número y su recíproco.
-La raíz cuadrada del doble de un número. s
-La tercera parte de la raíz cúbica de un número. 
-La cuarta potencia de un número más cuatro. 
-El cuadrado de un número más 10</t>
-  </si>
-  <si>
     <t>Identifica el dominio de la función</t>
   </si>
   <si>
@@ -579,12 +564,6 @@
     <t>Interactivo que muestra representaciones de funciones lineales y afines</t>
   </si>
   <si>
-    <t xml:space="preserve">Las funciones afines </t>
-  </si>
-  <si>
-    <t>Interactivo para reconocer las características y la expresión de las funciones afines</t>
-  </si>
-  <si>
     <t>Actividad para practicar la representación de funciones lineales y afines</t>
   </si>
   <si>
@@ -717,12 +696,6 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t>Competencias: situaciones que se modelan con funciones lineales y cuadráticas</t>
-  </si>
-  <si>
-    <t>Actividad que propone realizar el analisis de situaciones que se modelan con funciones lineales y cuadráticas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Evaluación </t>
   </si>
   <si>
@@ -810,9 +783,6 @@
     <t>RM_01_01_CO</t>
   </si>
   <si>
-    <t>Recurso M3A-01</t>
-  </si>
-  <si>
     <t>Recursos M aleatorios y diaporama F1</t>
   </si>
   <si>
@@ -837,9 +807,6 @@
     <t>Recurso M101A-01</t>
   </si>
   <si>
-    <t>Recurso F6B-01</t>
-  </si>
-  <si>
     <t>Recurso M101A-02</t>
   </si>
   <si>
@@ -874,6 +841,21 @@
   </si>
   <si>
     <t>24 recursos M</t>
+  </si>
+  <si>
+    <t>Interactivo que repasa el concepto de depemdencia lineal</t>
+  </si>
+  <si>
+    <t>Competencias: practica de las ecuaciones de una recta</t>
+  </si>
+  <si>
+    <t>Actividad que propone establecer las ecuaciones de las rectas que corresponden a las medianas de un triángulo. Relaciona pensamientos variacional y espacial</t>
+  </si>
+  <si>
+    <t>Interactivo que muestra la representación de funiones lineales y cuadráticas</t>
+  </si>
+  <si>
+    <t>Actividad para practica la representación de rectas y parábolas con Geogebra</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1146,9 +1128,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1176,16 +1155,41 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1226,31 +1230,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1556,11 +1535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V288"/>
+  <dimension ref="A1:V286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,82 +1568,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="27" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="53"/>
+      <c r="N1" s="61"/>
       <c r="O1" s="41" t="s">
         <v>109</v>
       </c>
       <c r="P1" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="56" t="s">
+      <c r="S1" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="58" t="s">
+      <c r="T1" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="56" t="s">
+      <c r="U1" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="32"/>
+      <c r="V1" s="31"/>
     </row>
     <row r="2" spans="1:22" s="27" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="48"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="56"/>
       <c r="M2" s="28" t="s">
         <v>90</v>
       </c>
@@ -1673,12 +1652,12 @@
       </c>
       <c r="O2" s="42"/>
       <c r="P2" s="42"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="32"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="31"/>
     </row>
     <row r="3" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1691,12 +1670,12 @@
         <v>123</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="21"/>
       <c r="G3" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H3" s="21">
         <v>1</v>
@@ -1716,22 +1695,22 @@
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
       <c r="O3" s="26"/>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R3" s="34" t="s">
+      <c r="Q3" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R3" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T3" s="35" t="s">
-        <v>214</v>
-      </c>
-      <c r="U3" s="33"/>
+      <c r="S3" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T3" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="U3" s="32"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -1751,14 +1730,14 @@
       <c r="G4" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <v>2</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1773,26 +1752,26 @@
       <c r="O4" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="33">
+      <c r="Q4" s="32">
         <v>6</v>
       </c>
-      <c r="R4" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S4" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="T4" s="36" t="s">
-        <v>222</v>
-      </c>
-      <c r="U4" s="33" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R4" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S4" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="T4" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="U4" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>15</v>
       </c>
@@ -1810,14 +1789,14 @@
       <c r="G5" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="21">
         <v>3</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>128</v>
+        <v>231</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1826,29 +1805,25 @@
         <v>8</v>
       </c>
       <c r="M5" s="8"/>
-      <c r="N5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="P5" s="31" t="s">
+      <c r="N5" s="29"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="33">
+      <c r="Q5" s="32">
         <v>6</v>
       </c>
-      <c r="R5" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S5" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="T5" s="36" t="s">
-        <v>224</v>
-      </c>
-      <c r="U5" s="33" t="s">
-        <v>223</v>
+      <c r="R5" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S5" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="U5" s="32" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1867,43 +1842,47 @@
       <c r="E6" s="13"/>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="30">
+        <v>4</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>130</v>
-      </c>
-      <c r="H6" s="31">
-        <v>4</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>240</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="P6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="33">
+      <c r="Q6" s="32">
         <v>6</v>
       </c>
-      <c r="R6" s="34" t="s">
+      <c r="R6" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="S6" s="33" t="s">
-        <v>225</v>
-      </c>
-      <c r="T6" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="U6" s="33" t="s">
-        <v>227</v>
+      <c r="S6" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="T6" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="U6" s="32" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1928,7 +1907,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>133</v>
@@ -1937,32 +1916,32 @@
         <v>20</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="O7" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="P7" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="33">
+      <c r="P7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="32">
         <v>6</v>
       </c>
-      <c r="R7" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="S7" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="T7" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="U7" s="33" t="s">
-        <v>231</v>
+      <c r="R7" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S7" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="T7" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="U7" s="32" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1978,19 +1957,21 @@
       <c r="D8" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="H8" s="31">
+        <v>233</v>
+      </c>
+      <c r="H8" s="30">
         <v>6</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>136</v>
+        <v>234</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -2000,131 +1981,129 @@
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="O8" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="P8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>6</v>
+      </c>
+      <c r="R8" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S8" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="T8" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="U8" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="H9" s="21">
+        <v>7</v>
+      </c>
+      <c r="I9" s="40"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="P9" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="39">
+        <v>10</v>
+      </c>
+      <c r="R9" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="S9" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="T9" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="U9" s="39" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="P8" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="33">
-        <v>6</v>
-      </c>
-      <c r="R8" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S8" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="T8" s="36" t="s">
-        <v>222</v>
-      </c>
-      <c r="U8" s="33" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="H9" s="31">
-        <v>7</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="P9" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="33">
-        <v>6</v>
-      </c>
-      <c r="R9" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S9" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="T9" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="U9" s="33" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="18"/>
       <c r="E10" s="13"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="62" t="s">
-        <v>209</v>
-      </c>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="64" t="s">
+      <c r="G10" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" s="30">
+        <v>8</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="64" t="s">
+      <c r="J10" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="63">
-        <v>10</v>
-      </c>
-      <c r="R10" s="63" t="s">
-        <v>205</v>
-      </c>
-      <c r="S10" s="63" t="s">
-        <v>206</v>
-      </c>
-      <c r="T10" s="63" t="s">
-        <v>209</v>
-      </c>
-      <c r="U10" s="63" t="s">
-        <v>207</v>
-      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="P10" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R10" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T10" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="U10" s="32"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
@@ -2137,21 +2116,21 @@
         <v>123</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="31">
-        <v>8</v>
+        <v>142</v>
+      </c>
+      <c r="H11" s="21">
+        <v>9</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -2161,25 +2140,23 @@
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="P11" s="31" t="s">
+      <c r="O11" s="9"/>
+      <c r="P11" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R11" s="34" t="s">
+      <c r="Q11" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R11" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S11" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T11" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="U11" s="33"/>
+      <c r="S11" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T11" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="U11" s="32"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
@@ -2192,51 +2169,47 @@
         <v>123</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="H12" s="21">
-        <v>9</v>
+        <v>141</v>
+      </c>
+      <c r="H12" s="30">
+        <v>10</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>55</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9"/>
-      <c r="P12" s="31" t="s">
+      <c r="P12" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="33">
-        <v>6</v>
-      </c>
-      <c r="R12" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="S12" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="T12" s="36" t="s">
-        <v>233</v>
-      </c>
-      <c r="U12" s="33" t="s">
-        <v>231</v>
-      </c>
+      <c r="Q12" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R12" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T12" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="U12" s="32"/>
     </row>
     <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
@@ -2249,47 +2222,47 @@
         <v>123</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="H13" s="21">
+        <v>11</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="17" t="s">
         <v>145</v>
-      </c>
-      <c r="H13" s="31">
-        <v>10</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="9"/>
-      <c r="P13" s="31" t="s">
+      <c r="P13" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="33" t="s">
+      <c r="Q13" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R13" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="S13" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T13" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="S13" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T13" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="U13" s="33"/>
+      <c r="U13" s="32"/>
     </row>
     <row r="14" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
@@ -2302,21 +2275,21 @@
         <v>123</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H14" s="31">
-        <v>11</v>
+        <v>147</v>
+      </c>
+      <c r="H14" s="30">
+        <v>12</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>19</v>
@@ -2327,22 +2300,22 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="9"/>
-      <c r="P14" s="31" t="s">
+      <c r="P14" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R14" s="34" t="s">
+      <c r="Q14" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R14" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S14" s="33" t="s">
+      <c r="S14" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T14" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="T14" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="U14" s="33"/>
+      <c r="U14" s="32"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
@@ -2355,15 +2328,15 @@
         <v>123</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="H15" s="31">
-        <v>12</v>
+        <v>149</v>
+      </c>
+      <c r="H15" s="21">
+        <v>13</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>20</v>
@@ -2380,22 +2353,22 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="9"/>
-      <c r="P15" s="31" t="s">
+      <c r="P15" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R15" s="34" t="s">
+      <c r="Q15" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R15" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S15" s="33" t="s">
-        <v>211</v>
+      <c r="S15" s="32" t="s">
+        <v>204</v>
       </c>
       <c r="T15" s="34" t="s">
-        <v>217</v>
-      </c>
-      <c r="U15" s="33"/>
+        <v>149</v>
+      </c>
+      <c r="U15" s="32"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
@@ -2408,47 +2381,47 @@
         <v>123</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="30">
+        <v>14</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="H16" s="21">
-        <v>13</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>153</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
-      <c r="P16" s="31" t="s">
+      <c r="P16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R16" s="34" t="s">
+      <c r="Q16" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R16" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S16" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T16" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="U16" s="33"/>
+      <c r="S16" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T16" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="U16" s="32"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
@@ -2461,21 +2434,21 @@
         <v>123</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="H17" s="31">
-        <v>14</v>
+        <v>153</v>
+      </c>
+      <c r="H17" s="21">
+        <v>15</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>19</v>
@@ -2486,22 +2459,22 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="9"/>
-      <c r="P17" s="31" t="s">
+      <c r="P17" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R17" s="34" t="s">
+      <c r="Q17" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R17" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S17" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T17" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="U17" s="33"/>
+      <c r="S17" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T17" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="U17" s="32"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2514,47 +2487,47 @@
         <v>123</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="H18" s="31">
-        <v>15</v>
+        <v>155</v>
+      </c>
+      <c r="H18" s="30">
+        <v>16</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="9"/>
-      <c r="P18" s="31" t="s">
+      <c r="P18" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R18" s="34" t="s">
+      <c r="Q18" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R18" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S18" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T18" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="U18" s="33"/>
+      <c r="S18" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T18" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="U18" s="32"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
@@ -2567,15 +2540,15 @@
         <v>123</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="H19" s="31">
-        <v>16</v>
+        <v>156</v>
+      </c>
+      <c r="H19" s="21">
+        <v>17</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>20</v>
@@ -2592,22 +2565,22 @@
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
       <c r="O19" s="9"/>
-      <c r="P19" s="31" t="s">
+      <c r="P19" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R19" s="34" t="s">
+      <c r="Q19" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R19" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S19" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T19" s="35" t="s">
-        <v>158</v>
-      </c>
-      <c r="U19" s="33"/>
+      <c r="S19" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T19" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="U19" s="32"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
@@ -2620,21 +2593,21 @@
         <v>123</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="H20" s="21">
-        <v>17</v>
+        <v>157</v>
+      </c>
+      <c r="H20" s="30">
+        <v>18</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>19</v>
@@ -2645,22 +2618,22 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
       <c r="O20" s="9"/>
-      <c r="P20" s="31" t="s">
+      <c r="P20" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R20" s="34" t="s">
+      <c r="Q20" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R20" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S20" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T20" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="U20" s="33"/>
+      <c r="S20" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T20" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="U20" s="32"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
@@ -2673,21 +2646,21 @@
         <v>123</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="H21" s="31">
-        <v>18</v>
+      <c r="H21" s="21">
+        <v>19</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>19</v>
@@ -2698,22 +2671,22 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="31" t="s">
+      <c r="P21" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R21" s="34" t="s">
+      <c r="Q21" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R21" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S21" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T21" s="35" t="s">
+      <c r="S21" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T21" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="U21" s="33"/>
+      <c r="U21" s="32"/>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2726,21 +2699,21 @@
         <v>123</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="H22" s="31">
-        <v>19</v>
+        <v>163</v>
+      </c>
+      <c r="H22" s="30">
+        <v>20</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>19</v>
@@ -2751,22 +2724,22 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
       <c r="O22" s="9"/>
-      <c r="P22" s="31" t="s">
+      <c r="P22" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R22" s="34" t="s">
+      <c r="Q22" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R22" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S22" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T22" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="U22" s="33"/>
+      <c r="S22" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T22" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="U22" s="32"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
@@ -2779,21 +2752,21 @@
         <v>123</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="H23" s="31">
-        <v>20</v>
+        <v>165</v>
+      </c>
+      <c r="H23" s="21">
+        <v>21</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>19</v>
@@ -2804,22 +2777,22 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="9"/>
-      <c r="P23" s="31" t="s">
+      <c r="P23" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R23" s="34" t="s">
+      <c r="Q23" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R23" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S23" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T23" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="U23" s="33"/>
+      <c r="S23" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T23" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="U23" s="32"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
@@ -2832,47 +2805,55 @@
         <v>123</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="E24" s="13"/>
+        <v>137</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="H24" s="21">
-        <v>21</v>
+        <v>167</v>
+      </c>
+      <c r="H24" s="30">
+        <v>22</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L24" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="31" t="s">
+      <c r="N24" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="P24" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R24" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="S24" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T24" s="35" t="s">
-        <v>168</v>
-      </c>
-      <c r="U24" s="33"/>
+      <c r="Q24" s="32">
+        <v>6</v>
+      </c>
+      <c r="R24" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S24" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="T24" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="U24" s="32" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
@@ -2885,18 +2866,18 @@
         <v>123</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="H25" s="31">
-        <v>22</v>
+      <c r="H25" s="21">
+        <v>23</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>171</v>
@@ -2905,27 +2886,29 @@
         <v>19</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
       <c r="O25" s="9"/>
-      <c r="P25" s="31" t="s">
+      <c r="P25" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R25" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="S25" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T25" s="35" t="s">
+      <c r="Q25" s="32">
+        <v>10</v>
+      </c>
+      <c r="R25" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="S25" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="T25" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="U25" s="33"/>
+      <c r="U25" s="32" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
@@ -2938,82 +2921,68 @@
         <v>123</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>139</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E26" s="13"/>
       <c r="F26" s="9"/>
       <c r="G26" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="H26" s="31">
-        <v>23</v>
+      <c r="H26" s="30">
+        <v>24</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>173</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M26" s="8"/>
-      <c r="N26" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O26" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="P26" s="31" t="s">
+      <c r="N26" s="8"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="33">
-        <v>6</v>
-      </c>
-      <c r="R26" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S26" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="T26" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="U26" s="33" t="s">
-        <v>223</v>
+      <c r="Q26" s="32">
+        <v>10</v>
+      </c>
+      <c r="R26" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="S26" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="T26" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="U26" s="32" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>175</v>
-      </c>
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="13"/>
       <c r="F27" s="9"/>
       <c r="G27" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="H27" s="31">
-        <v>24</v>
+        <v>205</v>
+      </c>
+      <c r="H27" s="21">
+        <v>25</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>19</v>
@@ -3024,157 +2993,179 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="9"/>
-      <c r="P27" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q27" s="33">
-        <v>10</v>
-      </c>
-      <c r="R27" s="34" t="s">
+      <c r="P27" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R27" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="S27" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T27" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="S27" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="T27" s="35" t="s">
-        <v>175</v>
-      </c>
-      <c r="U27" s="33" t="s">
-        <v>207</v>
-      </c>
+      <c r="U27" s="32"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>175</v>
-      </c>
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="13"/>
       <c r="F28" s="9"/>
       <c r="G28" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="H28" s="21">
-        <v>25</v>
+        <v>206</v>
+      </c>
+      <c r="H28" s="30">
+        <v>26</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>178</v>
+        <v>241</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="9"/>
-      <c r="P28" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q28" s="33">
-        <v>10</v>
-      </c>
-      <c r="R28" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="S28" s="33" t="s">
+      <c r="P28" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R28" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="S28" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="T28" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="T28" s="35" t="s">
-        <v>177</v>
-      </c>
-      <c r="U28" s="33" t="s">
-        <v>207</v>
-      </c>
+      <c r="U28" s="32"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="15"/>
+      <c r="A29" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>170</v>
+      </c>
       <c r="E29" s="13"/>
       <c r="F29" s="9"/>
       <c r="G29" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="17"/>
+        <v>174</v>
+      </c>
+      <c r="H29" s="21">
+        <v>27</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>175</v>
+      </c>
       <c r="K29" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R29" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="S29" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T29" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="U29" s="33"/>
+      <c r="P29" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q29" s="32">
+        <v>10</v>
+      </c>
+      <c r="R29" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="S29" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="T29" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="U29" s="32" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="15"/>
+      <c r="B30" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>170</v>
+      </c>
       <c r="E30" s="13"/>
       <c r="F30" s="9"/>
       <c r="G30" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="17"/>
+        <v>182</v>
+      </c>
+      <c r="H30" s="30">
+        <v>28</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="K30" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N30" s="8"/>
+      <c r="O30" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="P30" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="L30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="R30" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="S30" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="T30" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="U30" s="33"/>
+      <c r="Q30" s="32">
+        <v>6</v>
+      </c>
+      <c r="R30" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="S30" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="T30" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="U30" s="32" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
@@ -3187,21 +3178,21 @@
         <v>123</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="9"/>
       <c r="G31" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="H31" s="31">
-        <v>26</v>
+        <v>176</v>
+      </c>
+      <c r="H31" s="21">
+        <v>29</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>19</v>
@@ -3212,27 +3203,29 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="9"/>
-      <c r="P31" s="31" t="s">
+      <c r="P31" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="33">
+      <c r="Q31" s="32">
         <v>10</v>
       </c>
-      <c r="R31" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="S31" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="T31" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="U31" s="33" t="s">
-        <v>207</v>
+      <c r="R31" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="S31" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="T31" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="U31" s="32" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="A32" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="B32" s="19" t="s">
         <v>122</v>
       </c>
@@ -3240,52 +3233,48 @@
         <v>123</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="9"/>
       <c r="G32" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="H32" s="31">
-        <v>27</v>
+        <v>178</v>
+      </c>
+      <c r="H32" s="30">
+        <v>30</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>54</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="M32" s="8"/>
       <c r="N32" s="8"/>
-      <c r="O32" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="P32" s="31" t="s">
+      <c r="O32" s="9"/>
+      <c r="P32" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="33">
-        <v>6</v>
-      </c>
-      <c r="R32" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="S32" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="T32" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="U32" s="33" t="s">
-        <v>231</v>
+      <c r="Q32" s="32">
+        <v>10</v>
+      </c>
+      <c r="R32" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="S32" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="T32" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="U32" s="32" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3299,48 +3288,52 @@
         <v>123</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="9"/>
       <c r="G33" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="H33" s="31">
-        <v>28</v>
+        <v>180</v>
+      </c>
+      <c r="H33" s="21">
+        <v>31</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M33" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="N33" s="8"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q33" s="33">
-        <v>10</v>
-      </c>
-      <c r="R33" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="S33" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="T33" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="U33" s="33" t="s">
-        <v>207</v>
+      <c r="O33" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="P33" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="32">
+        <v>6</v>
+      </c>
+      <c r="R33" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S33" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="T33" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="U33" s="32" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3354,21 +3347,23 @@
         <v>123</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E34" s="13"/>
+        <v>170</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="F34" s="9"/>
       <c r="G34" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="H34" s="21">
-        <v>29</v>
+        <v>185</v>
+      </c>
+      <c r="H34" s="30">
+        <v>32</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>19</v>
@@ -3379,23 +3374,23 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="9"/>
-      <c r="P34" s="31" t="s">
+      <c r="P34" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="33">
+      <c r="Q34" s="32">
         <v>10</v>
       </c>
-      <c r="R34" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="S34" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="T34" s="35" t="s">
-        <v>183</v>
-      </c>
-      <c r="U34" s="33" t="s">
-        <v>207</v>
+      <c r="R34" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="S34" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="T34" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="U34" s="32" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3409,52 +3404,52 @@
         <v>123</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="9"/>
       <c r="G35" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="H35" s="31">
-        <v>30</v>
+        <v>238</v>
+      </c>
+      <c r="H35" s="21">
+        <v>33</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>186</v>
+        <v>239</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="N35" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8" t="s">
+        <v>120</v>
+      </c>
       <c r="O35" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="P35" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q35" s="33">
+        <v>195</v>
+      </c>
+      <c r="P35" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q35" s="32">
         <v>6</v>
       </c>
-      <c r="R35" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S35" s="33" t="s">
-        <v>225</v>
-      </c>
-      <c r="T35" s="37" t="s">
-        <v>236</v>
-      </c>
-      <c r="U35" s="33" t="s">
-        <v>227</v>
+      <c r="R35" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S35" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="T35" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="U35" s="32" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3468,51 +3463,39 @@
         <v>123</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>139</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="E36" s="13"/>
       <c r="F36" s="9"/>
       <c r="G36" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="H36" s="31">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="H36" s="30">
+        <v>34</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="9"/>
-      <c r="P36" s="31" t="s">
+      <c r="P36" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q36" s="33">
-        <v>10</v>
-      </c>
-      <c r="R36" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="S36" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="T36" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="U36" s="33" t="s">
-        <v>207</v>
-      </c>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="33"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="34"/>
+      <c r="U36" s="32"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
@@ -3530,16 +3513,16 @@
       <c r="E37" s="13"/>
       <c r="F37" s="9"/>
       <c r="G37" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="H37" s="31">
-        <v>32</v>
+        <v>188</v>
+      </c>
+      <c r="H37" s="21">
+        <v>35</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>20</v>
@@ -3549,133 +3532,103 @@
       </c>
       <c r="M37" s="8"/>
       <c r="N37" s="8" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="P37" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="P37" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q37" s="33">
+      <c r="Q37" s="32">
         <v>6</v>
       </c>
-      <c r="R37" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S37" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="T37" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="U37" s="33" t="s">
-        <v>223</v>
+      <c r="R37" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S37" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="T37" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="U37" s="32" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>199</v>
-      </c>
+      <c r="A38" s="4"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
       <c r="E38" s="13"/>
       <c r="F38" s="9"/>
       <c r="G38" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="21">
-        <v>33</v>
+        <v>191</v>
+      </c>
+      <c r="H38" s="30">
+        <v>36</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K38" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q38" s="33"/>
-      <c r="R38" s="34"/>
-      <c r="S38" s="33"/>
-      <c r="T38" s="35"/>
-      <c r="U38" s="33"/>
+      <c r="N38" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O38" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="P38" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q38" s="32">
+        <v>6</v>
+      </c>
+      <c r="R38" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="S38" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="T38" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="U38" s="32" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>199</v>
-      </c>
+      <c r="A39" s="4"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15"/>
       <c r="E39" s="13"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="H39" s="31">
-        <v>34</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="G39" s="16"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="6"/>
       <c r="M39" s="8"/>
-      <c r="N39" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="O39" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="P39" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q39" s="33">
-        <v>6</v>
-      </c>
-      <c r="R39" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S39" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="T39" s="37" t="s">
-        <v>222</v>
-      </c>
-      <c r="U39" s="33" t="s">
-        <v>223</v>
-      </c>
+      <c r="N39" s="8"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="32"/>
+      <c r="R39" s="33"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="34"/>
+      <c r="U39" s="32"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
@@ -3684,49 +3637,21 @@
       <c r="D40" s="15"/>
       <c r="E40" s="13"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="H40" s="31">
-        <v>35</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J40" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="6"/>
       <c r="M40" s="8"/>
-      <c r="N40" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O40" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="P40" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q40" s="33">
-        <v>6</v>
-      </c>
-      <c r="R40" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="S40" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="T40" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="U40" s="33" t="s">
-        <v>223</v>
-      </c>
+      <c r="N40" s="8"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="32"/>
+      <c r="R40" s="33"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="34"/>
+      <c r="U40" s="32"/>
     </row>
     <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
@@ -3745,11 +3670,11 @@
       <c r="N41" s="8"/>
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="34"/>
-      <c r="S41" s="33"/>
-      <c r="T41" s="35"/>
-      <c r="U41" s="33"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="33"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="34"/>
+      <c r="U41" s="32"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
@@ -3768,11 +3693,11 @@
       <c r="N42" s="8"/>
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
-      <c r="Q42" s="33"/>
-      <c r="R42" s="34"/>
-      <c r="S42" s="33"/>
-      <c r="T42" s="35"/>
-      <c r="U42" s="33"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="12"/>
+      <c r="U42" s="10"/>
     </row>
     <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
@@ -3784,18 +3709,20 @@
       <c r="G43" s="16"/>
       <c r="H43" s="9"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="17"/>
+      <c r="J43" s="17" t="s">
+        <v>235</v>
+      </c>
       <c r="K43" s="7"/>
       <c r="L43" s="6"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
       <c r="O43" s="9"/>
       <c r="P43" s="9"/>
-      <c r="Q43" s="33"/>
-      <c r="R43" s="34"/>
-      <c r="S43" s="33"/>
-      <c r="T43" s="35"/>
-      <c r="U43" s="33"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="12"/>
+      <c r="U43" s="10"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
@@ -3807,7 +3734,9 @@
       <c r="G44" s="16"/>
       <c r="H44" s="9"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="17"/>
+      <c r="J44" s="17" t="s">
+        <v>236</v>
+      </c>
       <c r="K44" s="7"/>
       <c r="L44" s="6"/>
       <c r="M44" s="8"/>
@@ -3830,9 +3759,7 @@
       <c r="G45" s="16"/>
       <c r="H45" s="9"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="17" t="s">
-        <v>244</v>
-      </c>
+      <c r="J45" s="17"/>
       <c r="K45" s="7"/>
       <c r="L45" s="6"/>
       <c r="M45" s="8"/>
@@ -3855,9 +3782,7 @@
       <c r="G46" s="16"/>
       <c r="H46" s="9"/>
       <c r="I46" s="5"/>
-      <c r="J46" s="17" t="s">
-        <v>245</v>
-      </c>
+      <c r="J46" s="17"/>
       <c r="K46" s="7"/>
       <c r="L46" s="6"/>
       <c r="M46" s="8"/>
@@ -4468,52 +4393,8 @@
       <c r="T72" s="12"/>
       <c r="U72" s="10"/>
     </row>
-    <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="17"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="8"/>
-      <c r="N73" s="8"/>
-      <c r="O73" s="9"/>
-      <c r="P73" s="9"/>
-      <c r="Q73" s="10"/>
-      <c r="R73" s="11"/>
-      <c r="S73" s="10"/>
-      <c r="T73" s="12"/>
-      <c r="U73" s="10"/>
-    </row>
-    <row r="74" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="17"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="8"/>
-      <c r="N74" s="8"/>
-      <c r="O74" s="9"/>
-      <c r="P74" s="9"/>
-      <c r="Q74" s="10"/>
-      <c r="R74" s="11"/>
-      <c r="S74" s="10"/>
-      <c r="T74" s="12"/>
-      <c r="U74" s="10"/>
-    </row>
+    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4525,193 +4406,193 @@
     <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
     </row>
     <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
         <v>115</v>
       </c>
     </row>
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4873,19 +4754,11 @@
     <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:U2">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4900,6 +4773,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4911,31 +4790,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N74</xm:sqref>
+          <xm:sqref>N3:N72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A74</xm:sqref>
+          <xm:sqref>A3:A72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I74 K3:K74 P3:P74</xm:sqref>
+          <xm:sqref>P3:P72 K3:K72 I3:I72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L74</xm:sqref>
+          <xm:sqref>L3:L72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M74</xm:sqref>
+          <xm:sqref>M3:M72</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Indicación de recursos aprovechados en escaleta mat 8 tema 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA MA_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA MA_08_07_CO.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="240">
   <si>
     <t>Asignatura</t>
   </si>
@@ -717,9 +717,6 @@
     <t>Mostrar situaciones que se modelan con funciones lineales y/o cuadráticas. Mostrar procesos de tabulación, representación, entre otras.</t>
   </si>
   <si>
-    <t>Explicar la modelación de situaciones con funciones lineales y cuadráticas. Dar objetivo de la actividad y proponer situaciones para que los estudiantes modelen mediante esas funciones</t>
-  </si>
-  <si>
     <t>Actividades que permitan evaluar lo trabajado en el tema sobre funciones, variación, funciones lineales y funciones cuadráticas</t>
   </si>
   <si>
@@ -814,9 +811,6 @@
   </si>
   <si>
     <t>Diaporama F1-01</t>
-  </si>
-  <si>
-    <t>Recurso M102AB-01</t>
   </si>
   <si>
     <t>Recurso M101AP-01</t>
@@ -1538,8 +1532,8 @@
   <dimension ref="A1:V286"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,7 +1664,7 @@
         <v>123</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="21"/>
@@ -1699,16 +1693,16 @@
         <v>19</v>
       </c>
       <c r="Q3" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R3" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T3" s="34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U3" s="32"/>
     </row>
@@ -1737,7 +1731,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1759,16 +1753,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="S4" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="S4" s="32" t="s">
+      <c r="T4" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="T4" s="35" t="s">
+      <c r="U4" s="32" t="s">
         <v>215</v>
-      </c>
-      <c r="U4" s="32" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1796,7 +1790,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1814,16 +1808,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S5" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="T5" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="T5" s="35" t="s">
+      <c r="U5" s="32" t="s">
         <v>218</v>
-      </c>
-      <c r="U5" s="32" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1873,16 +1867,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="S6" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="S6" s="32" t="s">
+      <c r="T6" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="T6" s="35" t="s">
+      <c r="U6" s="32" t="s">
         <v>222</v>
-      </c>
-      <c r="U6" s="32" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1932,16 +1926,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="S7" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="S7" s="32" t="s">
+      <c r="T7" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="T7" s="35" t="s">
+      <c r="U7" s="32" t="s">
         <v>215</v>
-      </c>
-      <c r="U7" s="32" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1962,7 +1956,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H8" s="30">
         <v>6</v>
@@ -1971,7 +1965,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1993,16 +1987,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="S8" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="S8" s="32" t="s">
-        <v>214</v>
-      </c>
       <c r="T8" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U8" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -2013,7 +2007,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="9"/>
       <c r="G9" s="38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H9" s="21">
         <v>7</v>
@@ -2029,7 +2023,7 @@
       <c r="M9" s="40"/>
       <c r="N9" s="40"/>
       <c r="O9" s="38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P9" s="39" t="s">
         <v>20</v>
@@ -2038,16 +2032,16 @@
         <v>10</v>
       </c>
       <c r="R9" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="S9" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="S9" s="39" t="s">
+      <c r="T9" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="U9" s="39" t="s">
         <v>199</v>
-      </c>
-      <c r="T9" s="39" t="s">
-        <v>202</v>
-      </c>
-      <c r="U9" s="39" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -2092,13 +2086,13 @@
         <v>19</v>
       </c>
       <c r="Q10" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R10" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S10" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T10" s="33" t="s">
         <v>138</v>
@@ -2145,16 +2139,16 @@
         <v>19</v>
       </c>
       <c r="Q11" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R11" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S11" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T11" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U11" s="32"/>
     </row>
@@ -2198,16 +2192,16 @@
         <v>19</v>
       </c>
       <c r="Q12" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R12" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S12" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T12" s="33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U12" s="32"/>
     </row>
@@ -2251,16 +2245,16 @@
         <v>19</v>
       </c>
       <c r="Q13" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R13" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S13" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T13" s="33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U13" s="32"/>
     </row>
@@ -2304,16 +2298,16 @@
         <v>19</v>
       </c>
       <c r="Q14" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R14" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S14" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T14" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U14" s="32"/>
     </row>
@@ -2357,13 +2351,13 @@
         <v>19</v>
       </c>
       <c r="Q15" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R15" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S15" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T15" s="34" t="s">
         <v>149</v>
@@ -2410,13 +2404,13 @@
         <v>19</v>
       </c>
       <c r="Q16" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R16" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S16" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T16" s="34" t="s">
         <v>151</v>
@@ -2463,13 +2457,13 @@
         <v>19</v>
       </c>
       <c r="Q17" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R17" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S17" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T17" s="34" t="s">
         <v>153</v>
@@ -2516,13 +2510,13 @@
         <v>19</v>
       </c>
       <c r="Q18" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R18" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S18" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T18" s="34" t="s">
         <v>155</v>
@@ -2569,13 +2563,13 @@
         <v>19</v>
       </c>
       <c r="Q19" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R19" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S19" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T19" s="34" t="s">
         <v>156</v>
@@ -2622,13 +2616,13 @@
         <v>19</v>
       </c>
       <c r="Q20" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R20" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S20" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T20" s="34" t="s">
         <v>157</v>
@@ -2675,13 +2669,13 @@
         <v>19</v>
       </c>
       <c r="Q21" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R21" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S21" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T21" s="34" t="s">
         <v>161</v>
@@ -2728,13 +2722,13 @@
         <v>19</v>
       </c>
       <c r="Q22" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R22" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S22" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T22" s="34" t="s">
         <v>163</v>
@@ -2781,13 +2775,13 @@
         <v>19</v>
       </c>
       <c r="Q23" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R23" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S23" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T23" s="34" t="s">
         <v>165</v>
@@ -2843,16 +2837,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="S24" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="S24" s="32" t="s">
-        <v>214</v>
-      </c>
       <c r="T24" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U24" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2898,16 +2892,16 @@
         <v>10</v>
       </c>
       <c r="R25" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="S25" s="32" t="s">
         <v>198</v>
-      </c>
-      <c r="S25" s="32" t="s">
-        <v>199</v>
       </c>
       <c r="T25" s="34" t="s">
         <v>170</v>
       </c>
       <c r="U25" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2953,16 +2947,16 @@
         <v>10</v>
       </c>
       <c r="R26" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="S26" s="32" t="s">
         <v>198</v>
-      </c>
-      <c r="S26" s="32" t="s">
-        <v>199</v>
       </c>
       <c r="T26" s="34" t="s">
         <v>172</v>
       </c>
       <c r="U26" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2973,7 +2967,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="9"/>
       <c r="G27" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H27" s="21">
         <v>25</v>
@@ -2982,7 +2976,7 @@
         <v>19</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>19</v>
@@ -2997,16 +2991,16 @@
         <v>20</v>
       </c>
       <c r="Q27" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R27" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S27" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="T27" s="34" t="s">
         <v>204</v>
-      </c>
-      <c r="T27" s="34" t="s">
-        <v>205</v>
       </c>
       <c r="U27" s="32"/>
     </row>
@@ -3018,7 +3012,7 @@
       <c r="E28" s="13"/>
       <c r="F28" s="9"/>
       <c r="G28" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H28" s="30">
         <v>26</v>
@@ -3027,7 +3021,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>19</v>
@@ -3042,16 +3036,16 @@
         <v>20</v>
       </c>
       <c r="Q28" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R28" s="33" t="s">
         <v>15</v>
       </c>
       <c r="S28" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T28" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="U28" s="32"/>
     </row>
@@ -3098,16 +3092,16 @@
         <v>10</v>
       </c>
       <c r="R29" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="S29" s="32" t="s">
         <v>198</v>
-      </c>
-      <c r="S29" s="32" t="s">
-        <v>199</v>
       </c>
       <c r="T29" s="34" t="s">
         <v>174</v>
       </c>
       <c r="U29" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3155,16 +3149,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="S30" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="S30" s="32" t="s">
-        <v>221</v>
-      </c>
       <c r="T30" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U30" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3210,16 +3204,16 @@
         <v>10</v>
       </c>
       <c r="R31" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="S31" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="S31" s="32" t="s">
+      <c r="T31" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="U31" s="32" t="s">
         <v>199</v>
-      </c>
-      <c r="T31" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="U31" s="32" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3265,16 +3259,16 @@
         <v>10</v>
       </c>
       <c r="R32" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="S32" s="32" t="s">
         <v>198</v>
-      </c>
-      <c r="S32" s="32" t="s">
-        <v>199</v>
       </c>
       <c r="T32" s="34" t="s">
         <v>178</v>
       </c>
       <c r="U32" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3324,16 +3318,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S33" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="T33" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U33" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3381,16 +3375,16 @@
         <v>10</v>
       </c>
       <c r="R34" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="S34" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="S34" s="32" t="s">
+      <c r="T34" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="U34" s="32" t="s">
         <v>199</v>
-      </c>
-      <c r="T34" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="U34" s="32" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3409,7 +3403,7 @@
       <c r="E35" s="13"/>
       <c r="F35" s="9"/>
       <c r="G35" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H35" s="21">
         <v>33</v>
@@ -3418,7 +3412,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3427,29 +3421,25 @@
         <v>8</v>
       </c>
       <c r="M35" s="8"/>
-      <c r="N35" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>195</v>
-      </c>
+      <c r="N35" s="8"/>
+      <c r="O35" s="9"/>
       <c r="P35" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="32">
-        <v>6</v>
+      <c r="Q35" s="32" t="s">
+        <v>202</v>
       </c>
       <c r="R35" s="33" t="s">
-        <v>213</v>
+        <v>15</v>
       </c>
       <c r="S35" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="T35" s="36" t="s">
-        <v>228</v>
+        <v>203</v>
+      </c>
+      <c r="T35" s="34" t="s">
+        <v>236</v>
       </c>
       <c r="U35" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3535,7 +3525,7 @@
         <v>33</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P37" s="30" t="s">
         <v>19</v>
@@ -3544,16 +3534,16 @@
         <v>6</v>
       </c>
       <c r="R37" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="S37" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="S37" s="32" t="s">
+      <c r="T37" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="T37" s="36" t="s">
+      <c r="U37" s="32" t="s">
         <v>215</v>
-      </c>
-      <c r="U37" s="32" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3586,7 +3576,7 @@
         <v>52</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P38" s="30" t="s">
         <v>20</v>
@@ -3595,16 +3585,16 @@
         <v>6</v>
       </c>
       <c r="R38" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="S38" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="S38" s="32" t="s">
-        <v>214</v>
-      </c>
       <c r="T38" s="36" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="U38" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3710,7 +3700,7 @@
       <c r="H43" s="9"/>
       <c r="I43" s="5"/>
       <c r="J43" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K43" s="7"/>
       <c r="L43" s="6"/>
@@ -3735,7 +3725,7 @@
       <c r="H44" s="9"/>
       <c r="I44" s="5"/>
       <c r="J44" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K44" s="7"/>
       <c r="L44" s="6"/>

</xml_diff>